<commit_message>
Schema almost done; Port Expander missing
</commit_message>
<xml_diff>
--- a/Projektdokumente und Unterlagen/ZeitplanSB.xlsx
+++ b/Projektdokumente und Unterlagen/ZeitplanSB.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
   <si>
     <t>soll</t>
   </si>
@@ -652,21 +652,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -680,6 +665,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1039,7 +1039,7 @@
   </sheetPr>
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="I13" sqref="I13"/>
     </sheetView>
@@ -1057,13 +1057,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="31.5">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
       <c r="H1" s="28"/>
@@ -1073,17 +1073,17 @@
     </row>
     <row r="2" spans="1:16" customFormat="1" ht="42" customHeight="1">
       <c r="C2" s="27"/>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="45" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="18" customHeight="1" thickBot="1">
       <c r="C3" s="36"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="42"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="46"/>
       <c r="F3" s="12">
         <v>44256</v>
       </c>
@@ -1119,10 +1119,10 @@
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="44">
-        <v>1</v>
-      </c>
-      <c r="B4" s="46" t="s">
+      <c r="A4" s="39">
+        <v>1</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -1150,8 +1150,8 @@
       <c r="P4" s="21"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="45"/>
-      <c r="B5" s="47"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1162,8 +1162,8 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="F5" s="30">
-        <v>1</v>
+      <c r="F5" s="30" t="s">
+        <v>4</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -1177,10 +1177,10 @@
       <c r="P5" s="22"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="44">
+      <c r="A6" s="39">
         <v>2</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="41" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -1210,8 +1210,8 @@
       <c r="P6" s="23"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="45"/>
-      <c r="B7" s="47"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
@@ -1239,10 +1239,10 @@
       <c r="P7" s="22"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="44">
+      <c r="A8" s="39">
         <v>3</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="41" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1272,8 +1272,8 @@
       <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="45"/>
-      <c r="B9" s="47"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1299,10 +1299,10 @@
       <c r="P9" s="22"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="44">
+      <c r="A10" s="39">
         <v>4</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1332,8 +1332,8 @@
       <c r="P10" s="23"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="45"/>
-      <c r="B11" s="47"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="7" t="s">
         <v>1</v>
       </c>
@@ -1342,12 +1342,16 @@
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1</v>
+      </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
@@ -1357,10 +1361,10 @@
       <c r="P11" s="22"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="44">
+      <c r="A12" s="39">
         <v>5</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="41" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -1388,8 +1392,8 @@
       <c r="P12" s="23"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="45"/>
-      <c r="B13" s="47"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="7" t="s">
         <v>1</v>
       </c>
@@ -1413,10 +1417,10 @@
       <c r="P13" s="22"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="44">
+      <c r="A14" s="39">
         <v>6</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="41" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1446,8 +1450,8 @@
       <c r="P14" s="23"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="45"/>
-      <c r="B15" s="47"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="42"/>
       <c r="C15" s="7" t="s">
         <v>1</v>
       </c>
@@ -1471,10 +1475,10 @@
       <c r="P15" s="22"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="44">
+      <c r="A16" s="39">
         <v>7</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="41" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1508,8 +1512,8 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="45"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="7" t="s">
         <v>1</v>
       </c>
@@ -1533,10 +1537,10 @@
       <c r="P17" s="22"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="44">
+      <c r="A18" s="39">
         <v>8</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="41" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -1564,8 +1568,8 @@
       <c r="P18" s="23"/>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="45"/>
-      <c r="B19" s="47"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="42"/>
       <c r="C19" s="7" t="s">
         <v>1</v>
       </c>
@@ -1589,10 +1593,10 @@
       <c r="P19" s="22"/>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="44">
+      <c r="A20" s="39">
         <v>9</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="41" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1622,8 +1626,8 @@
       <c r="P20" s="33"/>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="45"/>
-      <c r="B21" s="47"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="7" t="s">
         <v>1</v>
       </c>
@@ -1647,10 +1651,10 @@
       <c r="P21" s="22"/>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="44">
+      <c r="A22" s="39">
         <v>10</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="41" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1680,8 +1684,8 @@
       <c r="P22" s="23"/>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="45"/>
-      <c r="B23" s="47"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="7" t="s">
         <v>1</v>
       </c>
@@ -1705,10 +1709,10 @@
       <c r="P23" s="22"/>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="44">
+      <c r="A24" s="39">
         <v>11</v>
       </c>
-      <c r="B24" s="46"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="6" t="s">
         <v>0</v>
       </c>
@@ -1732,8 +1736,8 @@
       <c r="P24" s="23"/>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="45"/>
-      <c r="B25" s="47"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="42"/>
       <c r="C25" s="7" t="s">
         <v>1</v>
       </c>
@@ -1757,10 +1761,10 @@
       <c r="P25" s="22"/>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="44">
+      <c r="A26" s="39">
         <v>12</v>
       </c>
-      <c r="B26" s="46"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="6" t="s">
         <v>0</v>
       </c>
@@ -1784,8 +1788,8 @@
       <c r="P26" s="23"/>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="45"/>
-      <c r="B27" s="47"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="7" t="s">
         <v>1</v>
       </c>
@@ -1809,10 +1813,10 @@
       <c r="P27" s="22"/>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="44">
+      <c r="A28" s="39">
         <v>14</v>
       </c>
-      <c r="B28" s="46"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="6" t="s">
         <v>0</v>
       </c>
@@ -1834,8 +1838,8 @@
       <c r="P28" s="23"/>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="45"/>
-      <c r="B29" s="47"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="7" t="s">
         <v>1</v>
       </c>
@@ -1857,10 +1861,10 @@
       <c r="P29" s="22"/>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="44">
+      <c r="A30" s="39">
         <v>15</v>
       </c>
-      <c r="B30" s="46"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="6" t="s">
         <v>0</v>
       </c>
@@ -1882,8 +1886,8 @@
       <c r="P30" s="23"/>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="45"/>
-      <c r="B31" s="47"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="42"/>
       <c r="C31" s="7" t="s">
         <v>1</v>
       </c>
@@ -1905,10 +1909,10 @@
       <c r="P31" s="22"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="44">
+      <c r="A32" s="39">
         <v>16</v>
       </c>
-      <c r="B32" s="46"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="6" t="s">
         <v>0</v>
       </c>
@@ -1930,8 +1934,8 @@
       <c r="P32" s="23"/>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="45"/>
-      <c r="B33" s="47"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="42"/>
       <c r="C33" s="7" t="s">
         <v>1</v>
       </c>
@@ -1953,10 +1957,10 @@
       <c r="P33" s="22"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="44">
+      <c r="A34" s="39">
         <v>17</v>
       </c>
-      <c r="B34" s="46"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="6" t="s">
         <v>0</v>
       </c>
@@ -1978,8 +1982,8 @@
       <c r="P34" s="23"/>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="45"/>
-      <c r="B35" s="47"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="42"/>
       <c r="C35" s="7" t="s">
         <v>1</v>
       </c>
@@ -2001,10 +2005,10 @@
       <c r="P35" s="22"/>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="44">
+      <c r="A36" s="39">
         <v>19</v>
       </c>
-      <c r="B36" s="46"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="6" t="s">
         <v>0</v>
       </c>
@@ -2026,8 +2030,8 @@
       <c r="P36" s="23"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="45"/>
-      <c r="B37" s="47"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="42"/>
       <c r="C37" s="7" t="s">
         <v>1</v>
       </c>
@@ -2049,10 +2053,10 @@
       <c r="P37" s="22"/>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="44">
+      <c r="A38" s="39">
         <v>20</v>
       </c>
-      <c r="B38" s="46"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="6" t="s">
         <v>0</v>
       </c>
@@ -2074,8 +2078,8 @@
       <c r="P38" s="23"/>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="45"/>
-      <c r="B39" s="47"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="42"/>
       <c r="C39" s="7" t="s">
         <v>1</v>
       </c>
@@ -2120,12 +2124,31 @@
   <sheetProtection selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="39">
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="A32:A33"/>
@@ -2134,31 +2157,12 @@
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
   </mergeCells>
   <conditionalFormatting sqref="F38:P38 F36:P36 F34:P34 F32:P32 F30:P30 F28:P28 F26:P26 F24:P24 F20:P20 F18:P18 F16:P16 F14:P14 F12:P12 F10:P10 F8:P8 F6:P6 F22:P22 F4:P4">
     <cfRule type="beginsWith" dxfId="3" priority="2" operator="beginsWith" text="M">

</xml_diff>

<commit_message>
PCB finished, ready to order
</commit_message>
<xml_diff>
--- a/Projektdokumente und Unterlagen/ZeitplanSB.xlsx
+++ b/Projektdokumente und Unterlagen/ZeitplanSB.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
   <si>
     <t>soll</t>
   </si>
@@ -652,6 +652,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -665,21 +680,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1041,7 +1041,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I13" sqref="I13"/>
+      <selection pane="topRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5"/>
@@ -1057,13 +1057,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="31.5">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
       <c r="F1" s="28"/>
       <c r="G1" s="28"/>
       <c r="H1" s="28"/>
@@ -1073,17 +1073,17 @@
     </row>
     <row r="2" spans="1:16" customFormat="1" ht="42" customHeight="1">
       <c r="C2" s="27"/>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="41" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="18" customHeight="1" thickBot="1">
       <c r="C3" s="36"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="46"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="42"/>
       <c r="F3" s="12">
         <v>44256</v>
       </c>
@@ -1119,10 +1119,10 @@
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="39">
-        <v>1</v>
-      </c>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="44">
+        <v>1</v>
+      </c>
+      <c r="B4" s="46" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -1150,8 +1150,8 @@
       <c r="P4" s="21"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5" s="40"/>
-      <c r="B5" s="42"/>
+      <c r="A5" s="45"/>
+      <c r="B5" s="47"/>
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1177,10 +1177,10 @@
       <c r="P5" s="22"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6" s="39">
+      <c r="A6" s="44">
         <v>2</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="46" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="17" t="s">
@@ -1210,8 +1210,8 @@
       <c r="P6" s="23"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="40"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="45"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="7" t="s">
         <v>1</v>
       </c>
@@ -1239,10 +1239,10 @@
       <c r="P7" s="22"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="39">
+      <c r="A8" s="44">
         <v>3</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="46" t="s">
         <v>22</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -1272,8 +1272,8 @@
       <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9" s="40"/>
-      <c r="B9" s="42"/>
+      <c r="A9" s="45"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="7" t="s">
         <v>1</v>
       </c>
@@ -1282,7 +1282,7 @@
       </c>
       <c r="E9" s="20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
@@ -1290,7 +1290,9 @@
         <v>1</v>
       </c>
       <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="J9" s="8">
+        <v>1</v>
+      </c>
       <c r="K9" s="8"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
@@ -1299,10 +1301,10 @@
       <c r="P9" s="22"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="39">
+      <c r="A10" s="44">
         <v>4</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="46" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1332,8 +1334,8 @@
       <c r="P10" s="23"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="40"/>
-      <c r="B11" s="42"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="7" t="s">
         <v>1</v>
       </c>
@@ -1342,7 +1344,7 @@
       </c>
       <c r="E11" s="20">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="8"/>
@@ -1352,7 +1354,9 @@
       <c r="I11" s="8">
         <v>1</v>
       </c>
-      <c r="J11" s="8"/>
+      <c r="J11" s="8" t="s">
+        <v>3</v>
+      </c>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
@@ -1361,10 +1365,10 @@
       <c r="P11" s="22"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="39">
+      <c r="A12" s="44">
         <v>5</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="46" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -1392,8 +1396,8 @@
       <c r="P12" s="23"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="40"/>
-      <c r="B13" s="42"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="7" t="s">
         <v>1</v>
       </c>
@@ -1417,10 +1421,10 @@
       <c r="P13" s="22"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="39">
+      <c r="A14" s="44">
         <v>6</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="46" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1450,8 +1454,8 @@
       <c r="P14" s="23"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="40"/>
-      <c r="B15" s="42"/>
+      <c r="A15" s="45"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="7" t="s">
         <v>1</v>
       </c>
@@ -1460,14 +1464,18 @@
       </c>
       <c r="E15" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="J15" s="8">
+        <v>1</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -1475,10 +1483,10 @@
       <c r="P15" s="22"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="39">
+      <c r="A16" s="44">
         <v>7</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="46" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="6" t="s">
@@ -1512,8 +1520,8 @@
       </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="40"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="7" t="s">
         <v>1</v>
       </c>
@@ -1537,10 +1545,10 @@
       <c r="P17" s="22"/>
     </row>
     <row r="18" spans="1:16">
-      <c r="A18" s="39">
+      <c r="A18" s="44">
         <v>8</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="46" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="6" t="s">
@@ -1568,8 +1576,8 @@
       <c r="P18" s="23"/>
     </row>
     <row r="19" spans="1:16">
-      <c r="A19" s="40"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="7" t="s">
         <v>1</v>
       </c>
@@ -1593,10 +1601,10 @@
       <c r="P19" s="22"/>
     </row>
     <row r="20" spans="1:16">
-      <c r="A20" s="39">
+      <c r="A20" s="44">
         <v>9</v>
       </c>
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="46" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="6" t="s">
@@ -1626,8 +1634,8 @@
       <c r="P20" s="33"/>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="40"/>
-      <c r="B21" s="42"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="7" t="s">
         <v>1</v>
       </c>
@@ -1651,10 +1659,10 @@
       <c r="P21" s="22"/>
     </row>
     <row r="22" spans="1:16">
-      <c r="A22" s="39">
+      <c r="A22" s="44">
         <v>10</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="46" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -1684,8 +1692,8 @@
       <c r="P22" s="23"/>
     </row>
     <row r="23" spans="1:16">
-      <c r="A23" s="40"/>
-      <c r="B23" s="42"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="7" t="s">
         <v>1</v>
       </c>
@@ -1709,10 +1717,10 @@
       <c r="P23" s="22"/>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="39">
+      <c r="A24" s="44">
         <v>11</v>
       </c>
-      <c r="B24" s="41"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="6" t="s">
         <v>0</v>
       </c>
@@ -1736,8 +1744,8 @@
       <c r="P24" s="23"/>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="40"/>
-      <c r="B25" s="42"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="7" t="s">
         <v>1</v>
       </c>
@@ -1761,10 +1769,10 @@
       <c r="P25" s="22"/>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="39">
+      <c r="A26" s="44">
         <v>12</v>
       </c>
-      <c r="B26" s="41"/>
+      <c r="B26" s="46"/>
       <c r="C26" s="6" t="s">
         <v>0</v>
       </c>
@@ -1788,8 +1796,8 @@
       <c r="P26" s="23"/>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="40"/>
-      <c r="B27" s="42"/>
+      <c r="A27" s="45"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="7" t="s">
         <v>1</v>
       </c>
@@ -1813,10 +1821,10 @@
       <c r="P27" s="22"/>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="39">
+      <c r="A28" s="44">
         <v>14</v>
       </c>
-      <c r="B28" s="41"/>
+      <c r="B28" s="46"/>
       <c r="C28" s="6" t="s">
         <v>0</v>
       </c>
@@ -1838,8 +1846,8 @@
       <c r="P28" s="23"/>
     </row>
     <row r="29" spans="1:16">
-      <c r="A29" s="40"/>
-      <c r="B29" s="42"/>
+      <c r="A29" s="45"/>
+      <c r="B29" s="47"/>
       <c r="C29" s="7" t="s">
         <v>1</v>
       </c>
@@ -1861,10 +1869,10 @@
       <c r="P29" s="22"/>
     </row>
     <row r="30" spans="1:16">
-      <c r="A30" s="39">
+      <c r="A30" s="44">
         <v>15</v>
       </c>
-      <c r="B30" s="41"/>
+      <c r="B30" s="46"/>
       <c r="C30" s="6" t="s">
         <v>0</v>
       </c>
@@ -1886,8 +1894,8 @@
       <c r="P30" s="23"/>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="40"/>
-      <c r="B31" s="42"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="7" t="s">
         <v>1</v>
       </c>
@@ -1909,10 +1917,10 @@
       <c r="P31" s="22"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="39">
+      <c r="A32" s="44">
         <v>16</v>
       </c>
-      <c r="B32" s="41"/>
+      <c r="B32" s="46"/>
       <c r="C32" s="6" t="s">
         <v>0</v>
       </c>
@@ -1934,8 +1942,8 @@
       <c r="P32" s="23"/>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="40"/>
-      <c r="B33" s="42"/>
+      <c r="A33" s="45"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="7" t="s">
         <v>1</v>
       </c>
@@ -1957,10 +1965,10 @@
       <c r="P33" s="22"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="39">
+      <c r="A34" s="44">
         <v>17</v>
       </c>
-      <c r="B34" s="41"/>
+      <c r="B34" s="46"/>
       <c r="C34" s="6" t="s">
         <v>0</v>
       </c>
@@ -1982,8 +1990,8 @@
       <c r="P34" s="23"/>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="40"/>
-      <c r="B35" s="42"/>
+      <c r="A35" s="45"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="7" t="s">
         <v>1</v>
       </c>
@@ -2005,10 +2013,10 @@
       <c r="P35" s="22"/>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="39">
+      <c r="A36" s="44">
         <v>19</v>
       </c>
-      <c r="B36" s="41"/>
+      <c r="B36" s="46"/>
       <c r="C36" s="6" t="s">
         <v>0</v>
       </c>
@@ -2030,8 +2038,8 @@
       <c r="P36" s="23"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="40"/>
-      <c r="B37" s="42"/>
+      <c r="A37" s="45"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="7" t="s">
         <v>1</v>
       </c>
@@ -2053,10 +2061,10 @@
       <c r="P37" s="22"/>
     </row>
     <row r="38" spans="1:16">
-      <c r="A38" s="39">
+      <c r="A38" s="44">
         <v>20</v>
       </c>
-      <c r="B38" s="41"/>
+      <c r="B38" s="46"/>
       <c r="C38" s="6" t="s">
         <v>0</v>
       </c>
@@ -2078,8 +2086,8 @@
       <c r="P38" s="23"/>
     </row>
     <row r="39" spans="1:16">
-      <c r="A39" s="40"/>
-      <c r="B39" s="42"/>
+      <c r="A39" s="45"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="7" t="s">
         <v>1</v>
       </c>
@@ -2124,31 +2132,12 @@
   <sheetProtection selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="39">
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="B38:B39"/>
     <mergeCell ref="A32:A33"/>
@@ -2157,12 +2146,31 @@
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="B36:B37"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="F38:P38 F36:P36 F34:P34 F32:P32 F30:P30 F28:P28 F26:P26 F24:P24 F20:P20 F18:P18 F16:P16 F14:P14 F12:P12 F10:P10 F8:P8 F6:P6 F22:P22 F4:P4">
     <cfRule type="beginsWith" dxfId="3" priority="2" operator="beginsWith" text="M">

</xml_diff>